<commit_message>
eta_time_estimate decorator not work ,bug need fix
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -359,52 +359,52 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="n">
-        <v>16.67632848847679</v>
+        <v>17.05443219947866</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="n">
-        <v>17.787315</v>
+        <v>17.11297689133074</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="n">
-        <v>16.10377599082324</v>
+        <v>16.78313955193191</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="n">
-        <v>17.70342</v>
+        <v>16.33713498461266</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="n">
-        <v>17.10808171922956</v>
+        <v>17.30922597452606</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="n">
-        <v>16.99813372930783</v>
+        <v>16.68082997295395</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="n">
-        <v>16.49457940583927</v>
+        <v>16.32995891797985</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="n">
-        <v>16.71986587891587</v>
+        <v>17.10101204440819</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="n">
-        <v>16.44046735958519</v>
+        <v>16.80536188956136</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="n">
-        <v>15.49382306193328</v>
+        <v>17.32481890889563</v>
       </c>
     </row>
   </sheetData>

</xml_diff>